<commit_message>
update error 1 pixel version
</commit_message>
<xml_diff>
--- a/Lab7/memory_index.xlsx
+++ b/Lab7/memory_index.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\125wi\OneDrive\桌面\verilog_place\verilog_practice\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6096B772-7B9B-41C4-A57D-367C76268155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6C0BDC-0BE5-4EA7-A550-4789918F6414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C1DD1A8B-5319-47F8-B4C5-79A8A0772AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="8x8" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -67,12 +68,42 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -81,11 +112,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -402,18 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61454B18-BD93-4C1C-9DA8-4D56963BB5C6}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="8" width="4.6328125" customWidth="1"/>
+    <col min="11" max="16" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>0</v>
       </c>
@@ -439,7 +477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>8</v>
       </c>
@@ -464,8 +502,26 @@
       <c r="H2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>16</v>
       </c>
@@ -490,8 +546,26 @@
       <c r="H3">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>24</v>
       </c>
@@ -516,8 +590,26 @@
       <c r="H4">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
+      <c r="M4">
+        <v>14</v>
+      </c>
+      <c r="N4">
+        <v>15</v>
+      </c>
+      <c r="O4">
+        <v>16</v>
+      </c>
+      <c r="P4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>32</v>
       </c>
@@ -542,8 +634,26 @@
       <c r="H5">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>19</v>
+      </c>
+      <c r="M5">
+        <v>20</v>
+      </c>
+      <c r="N5">
+        <v>21</v>
+      </c>
+      <c r="O5">
+        <v>22</v>
+      </c>
+      <c r="P5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>40</v>
       </c>
@@ -568,8 +678,26 @@
       <c r="H6">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <v>24</v>
+      </c>
+      <c r="L6">
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <v>26</v>
+      </c>
+      <c r="N6">
+        <v>27</v>
+      </c>
+      <c r="O6">
+        <v>28</v>
+      </c>
+      <c r="P6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>48</v>
       </c>
@@ -594,8 +722,26 @@
       <c r="H7">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>31</v>
+      </c>
+      <c r="M7">
+        <v>32</v>
+      </c>
+      <c r="N7">
+        <v>33</v>
+      </c>
+      <c r="O7">
+        <v>34</v>
+      </c>
+      <c r="P7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>56</v>
       </c>
@@ -621,6 +767,53 @@
         <v>63</v>
       </c>
     </row>
+    <row r="10" spans="1:16" ht="17.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="3">
+        <f>FLOOR($A$12/6,1)*8+0+MOD($A$12,6)</f>
+        <v>13</v>
+      </c>
+      <c r="D11" s="3">
+        <f>FLOOR($A$12/6,1)*8+1+MOD($A$12,6)</f>
+        <v>14</v>
+      </c>
+      <c r="E11" s="3">
+        <f>FLOOR($A$12/6,1)*8+2+MOD($A$12,6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <f>FLOOR($A$12/6,1)*8+8+MOD($A$12,6)</f>
+        <v>21</v>
+      </c>
+      <c r="D12" s="3">
+        <f>FLOOR($A$12/6,1)*8+9+MOD($A$12,6)</f>
+        <v>22</v>
+      </c>
+      <c r="E12" s="3">
+        <f>FLOOR($A$12/6,1)*8+10+MOD($A$12,6)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="3">
+        <f>FLOOR($A$12/6,1)*8+16+MOD($A$12,6)</f>
+        <v>29</v>
+      </c>
+      <c r="D13" s="3">
+        <f>FLOOR($A$12/6,1)*8+17+MOD($A$12,6)</f>
+        <v>30</v>
+      </c>
+      <c r="E13" s="3">
+        <f>FLOOR($A$12/6,1)*8+18+MOD($A$12,6)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17.5" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update lab7 reference excel
</commit_message>
<xml_diff>
--- a/Lab7/memory_index.xlsx
+++ b/Lab7/memory_index.xlsx
@@ -8,28 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\125wi\OneDrive\桌面\verilog_place\verilog_practice\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E35004-0873-4250-AB7F-0222442FCC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0886C-DCEC-486C-925C-569492AFD88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C1DD1A8B-5319-47F8-B4C5-79A8A0772AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="8x8" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -442,7 +431,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -771,46 +760,46 @@
     <row r="11" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <f>FLOOR($A$12/6,1)*8+0+MOD($A$12,6)</f>
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3">
         <f>FLOOR($A$12/6,1)*8+1+MOD($A$12,6)</f>
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3">
         <f>FLOOR($A$12/6,1)*8+2+MOD($A$12,6)</f>
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <f>FLOOR($A$12/6,1)*8+8+MOD($A$12,6)</f>
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3">
         <f>FLOOR($A$12/6,1)*8+9+MOD($A$12,6)</f>
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3">
         <f>FLOOR($A$12/6,1)*8+10+MOD($A$12,6)</f>
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <f>FLOOR($A$12/6,1)*8+16+MOD($A$12,6)</f>
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3">
         <f>FLOOR($A$12/6,1)*8+17+MOD($A$12,6)</f>
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E13" s="3">
         <f>FLOOR($A$12/6,1)*8+18+MOD($A$12,6)</f>
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="17.5" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>